<commit_message>
0.00 MPa bug fixed
</commit_message>
<xml_diff>
--- a/utilities/Dividers_calculator.xlsx
+++ b/utilities/Dividers_calculator.xlsx
@@ -5,7 +5,7 @@
   <fileSharing readOnlyRecommended="0" userName="alexe"/>
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="2" xWindow="240" yWindow="60" windowWidth="0" windowHeight="0" tabRatio="500"/>
+    <workbookView activeTab="0" xWindow="240" yWindow="60" windowWidth="0" windowHeight="0" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="1-5 V" sheetId="1" r:id="rId4"/>
@@ -15,17 +15,17 @@
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1638603799" val="982" rev="124" revOS="4" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1638603799" fixedDigits="0" showNotice="1" showProtection="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1638603799"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1638603799"/>
+      <pm:revision xmlns:pm="smNativeData" day="1638789380" val="982" rev="124" revOS="4" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1638789380" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1638789380" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1638789380"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="26">
   <si>
     <t>Upper R</t>
   </si>
@@ -109,7 +109,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="12">
+  <numFmts count="13">
     <numFmt numFmtId="5" formatCode="#,##0\ &quot;$&quot;;\-#,##0\ &quot;$&quot;"/>
     <numFmt numFmtId="6" formatCode="#,##0\ &quot;$&quot;;[Red]\-#,##0\ &quot;$&quot;"/>
     <numFmt numFmtId="7" formatCode="#,##0.00\ &quot;$&quot;;\-#,##0.00\ &quot;$&quot;"/>
@@ -122,6 +122,7 @@
     <numFmt numFmtId="1" formatCode="0"/>
     <numFmt numFmtId="164" formatCode="0.000000"/>
     <numFmt numFmtId="165" formatCode="0.000000000"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -132,7 +133,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1638603799" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1638789380" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -149,7 +150,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1638603799" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1638789380" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default" weight="bold"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -171,7 +172,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1638603799" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1638789380" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -193,7 +194,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1638603799"/>
+          <pm:border xmlns:pm="smNativeData" id="1638789380"/>
         </ext>
       </extLst>
     </border>
@@ -212,7 +213,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1638603799"/>
+          <pm:border xmlns:pm="smNativeData" id="1638789380"/>
         </ext>
       </extLst>
     </border>
@@ -220,13 +221,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
@@ -234,7 +236,7 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1638603799" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1638789380" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
     </ext>
@@ -498,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView view="normal" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:C22"/>
+    <sheetView tabSelected="1" view="normal" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="13.45"/>
@@ -609,10 +611,16 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="2:2">
+    <row r="10" spans="2:6">
       <c r="B10" s="4"/>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="E10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -623,8 +631,15 @@
       <c r="C11" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="E11" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="F11" s="6">
+        <f>E11*B$11</f>
+        <v>0.60714285714285694</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -635,8 +650,15 @@
       <c r="C12" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="1:3">
+      <c r="E12" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="F12" s="6">
+        <f>E12*B$11</f>
+        <v>1.21428571428571397</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -647,8 +669,15 @@
       <c r="C13" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="1:2">
+      <c r="E13" s="6" t="n">
+        <v>2.58000000000000007</v>
+      </c>
+      <c r="F13" s="6">
+        <f>E13*B$11</f>
+        <v>1.5664285714285711</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -656,8 +685,15 @@
         <f>B12*B6*B9/B3</f>
         <v>96459.9134199133405</v>
       </c>
-    </row>
-    <row r="15" spans="1:2">
+      <c r="E14" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="F14" s="6">
+        <f>E14*B$11</f>
+        <v>2.42857142857142794</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -665,11 +701,20 @@
         <f>B13*B6*B9/B3</f>
         <v>482299.567099566688</v>
       </c>
-    </row>
-    <row r="16" spans="2:2">
+      <c r="E15" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="F15" s="6">
+        <f>E15*B$11</f>
+        <v>3.0357142857142847</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6">
       <c r="B16" s="4"/>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -677,8 +722,10 @@
         <f>(B8-B7)/(B15-B14)</f>
         <v>0.0000259175020105698328</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -686,6 +733,11 @@
         <f>(B8*B14-B7*B15)/(B14-B15)</f>
         <v>-2.49999999999999734</v>
       </c>
+      <c r="E18" s="6">
+        <f>B1/(B1+B2)</f>
+        <v>0.392857142857142847</v>
+      </c>
+      <c r="F18" s="6"/>
     </row>
     <row r="19" spans="2:2">
       <c r="B19" s="4"/>
@@ -754,7 +806,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1638603799" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1638789380" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -763,16 +815,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1638603799" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1638603799" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1638603799" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1638603799" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1638789380" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1638789380" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1638789380" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1638789380" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1638603799" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1638789380" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -1002,7 +1054,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1638603799" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1638789380" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1011,16 +1063,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1638603799" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1638603799" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1638603799" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1638603799" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1638789380" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1638789380" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1638789380" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1638789380" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1638603799" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1638789380" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -1033,7 +1085,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="normal" workbookViewId="0">
+    <sheetView view="normal" workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -1251,7 +1303,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1638603799" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1638789380" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1260,16 +1312,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1638603799" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1638603799" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1638603799" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1638603799" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1638789380" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1638789380" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1638789380" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1638789380" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1638603799" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1638789380" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>

<commit_message>
Concentrator buzz bug fixed rumgV0_900.hex
</commit_message>
<xml_diff>
--- a/utilities/Dividers_calculator.xlsx
+++ b/utilities/Dividers_calculator.xlsx
@@ -15,10 +15,10 @@
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1638789380" val="982" rev="124" revOS="4" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1638789380" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1638789380" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1638789380"/>
+      <pm:revision xmlns:pm="smNativeData" day="1638791020" val="982" rev="124" revOS="4" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1638791020" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1638791020" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1638791020"/>
     </ext>
   </extLst>
 </workbook>
@@ -133,7 +133,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1638789380" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1638791020" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -150,7 +150,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1638789380" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1638791020" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default" weight="bold"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -172,7 +172,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1638789380" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1638791020" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -194,7 +194,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1638789380"/>
+          <pm:border xmlns:pm="smNativeData" id="1638791020"/>
         </ext>
       </extLst>
     </border>
@@ -213,7 +213,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1638789380"/>
+          <pm:border xmlns:pm="smNativeData" id="1638791020"/>
         </ext>
       </extLst>
     </border>
@@ -236,7 +236,7 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1638789380" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1638791020" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
     </ext>
@@ -670,11 +670,11 @@
         <v>4</v>
       </c>
       <c r="E13" s="6" t="n">
-        <v>2.58000000000000007</v>
+        <v>3</v>
       </c>
       <c r="F13" s="6">
         <f>E13*B$11</f>
-        <v>1.5664285714285711</v>
+        <v>1.821428571428571</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -806,7 +806,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1638789380" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1638791020" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -815,16 +815,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1638789380" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1638789380" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1638789380" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1638789380" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1638791020" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1638791020" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1638791020" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1638791020" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1638789380" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1638791020" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -1054,7 +1054,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1638789380" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1638791020" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1063,16 +1063,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1638789380" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1638789380" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1638789380" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1638789380" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1638791020" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1638791020" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1638791020" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1638791020" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1638789380" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1638791020" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -1303,7 +1303,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1638789380" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1638791020" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1312,16 +1312,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1638789380" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1638789380" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1638789380" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1638789380" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1638791020" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1638791020" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1638791020" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1638791020" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1638789380" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1638791020" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>

<commit_message>
1 kOhm sensor output impedance corrected  V 0.906
</commit_message>
<xml_diff>
--- a/utilities/Dividers_calculator.xlsx
+++ b/utilities/Dividers_calculator.xlsx
@@ -15,22 +15,25 @@
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1638791020" val="982" rev="124" revOS="4" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1638791020" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1638791020" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1638791020"/>
+      <pm:revision xmlns:pm="smNativeData" day="1638877689" val="982" rev="124" revOS="4" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1638877689" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1638877689" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1638877689"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="27">
+  <si>
+    <t>Ouput impedance</t>
+  </si>
+  <si>
+    <t>Ohm</t>
+  </si>
   <si>
     <t>Upper R</t>
-  </si>
-  <si>
-    <t>Ohm</t>
   </si>
   <si>
     <t>Lower R</t>
@@ -133,7 +136,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1638791020" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1638877689" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -150,7 +153,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1638791020" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1638877689" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default" weight="bold"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -172,7 +175,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1638791020" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1638877689" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -194,7 +197,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1638791020"/>
+          <pm:border xmlns:pm="smNativeData" id="1638877689"/>
         </ext>
       </extLst>
     </border>
@@ -213,7 +216,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1638791020"/>
+          <pm:border xmlns:pm="smNativeData" id="1638877689"/>
         </ext>
       </extLst>
     </border>
@@ -236,7 +239,7 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1638791020" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1638877689" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
     </ext>
@@ -500,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView tabSelected="1" view="normal" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E11" sqref="E11:F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="13.45"/>
@@ -517,7 +520,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="n">
-        <v>3300</v>
+        <v>1000</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>1</v>
@@ -528,7 +531,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="n">
-        <v>5100</v>
+        <v>3300</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>1</v>
@@ -539,21 +542,21 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>3.29999999999999982</v>
+        <v>5100</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1" t="n">
-        <v>1</v>
+        <v>3.29999999999999982</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -561,167 +564,138 @@
         <v>6</v>
       </c>
       <c r="B5" s="1" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="2" t="n">
-        <v>4096</v>
+      <c r="B6" s="1" t="n">
+        <v>5</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>4096</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="B7" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="B8" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="2" t="n">
+      <c r="B9" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="2" t="n">
         <v>128</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6">
-      <c r="B10" s="4"/>
-      <c r="E10" t="s">
-        <v>4</v>
-      </c>
-      <c r="F10" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" t="s">
+      <c r="C10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="4">
-        <f>B2/(B1+B2)</f>
-        <v>0.607142857142857117</v>
-      </c>
-      <c r="C11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="F11" s="6">
-        <f>E11*B$11</f>
-        <v>0.60714285714285694</v>
-      </c>
+    </row>
+    <row r="11" spans="2:6">
+      <c r="B11" s="4"/>
+      <c r="E11"/>
+      <c r="F11"/>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="4">
+        <f>B3/(B2+B3+B1)</f>
+        <v>0.54255319148936163</v>
+      </c>
+      <c r="C12" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="4">
-        <f>B4*B11</f>
-        <v>0.60714285714285694</v>
-      </c>
-      <c r="C12" t="s">
-        <v>4</v>
-      </c>
-      <c r="E12" s="6" t="n">
-        <v>2</v>
-      </c>
-      <c r="F12" s="6">
-        <f>E12*B$11</f>
-        <v>1.21428571428571397</v>
-      </c>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>17</v>
       </c>
       <c r="B13" s="4">
-        <f>B5*B11</f>
-        <v>3.0357142857142847</v>
+        <f>B5*B12</f>
+        <v>0.542553191489361986</v>
       </c>
       <c r="C13" t="s">
-        <v>4</v>
-      </c>
-      <c r="E13" s="6" t="n">
-        <v>3</v>
-      </c>
-      <c r="F13" s="6">
-        <f>E13*B$11</f>
-        <v>1.821428571428571</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="2">
-        <f>B12*B6*B9/B3</f>
-        <v>96459.9134199133405</v>
-      </c>
-      <c r="E14" s="6" t="n">
-        <v>4</v>
-      </c>
-      <c r="F14" s="6">
-        <f>E14*B$11</f>
-        <v>2.42857142857142794</v>
-      </c>
+      <c r="B14" s="4">
+        <f>B6*B12</f>
+        <v>2.71276595744680993</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>19</v>
       </c>
       <c r="B15" s="2">
-        <f>B13*B6*B9/B3</f>
-        <v>482299.567099566688</v>
-      </c>
-      <c r="E15" s="6" t="n">
-        <v>5</v>
-      </c>
-      <c r="F15" s="6">
-        <f>E15*B$11</f>
-        <v>3.0357142857142847</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6">
-      <c r="B16" s="4"/>
+        <f>B13*B7*B10/B4</f>
+        <v>86198.2205029015313</v>
+      </c>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="2">
+        <f>B14*B7*B10/B4</f>
+        <v>430991.102514506085</v>
+      </c>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="1:6">
-      <c r="A17" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" s="5">
-        <f>(B8-B7)/(B15-B14)</f>
-        <v>0.0000259175020105698328</v>
-      </c>
+    <row r="17" spans="2:6">
+      <c r="B17" s="4"/>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
     </row>
@@ -729,45 +703,50 @@
       <c r="A18" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="4">
-        <f>(B8*B14-B7*B15)/(B14-B15)</f>
-        <v>-2.49999999999999734</v>
-      </c>
-      <c r="E18" s="6">
-        <f>B1/(B1+B2)</f>
-        <v>0.392857142857142847</v>
-      </c>
+      <c r="B18" s="5">
+        <f>(B9-B8)/(B16-B15)</f>
+        <v>0.0000290029189165901045</v>
+      </c>
+      <c r="E18" s="6"/>
       <c r="F18" s="6"/>
     </row>
-    <row r="19" spans="2:2">
-      <c r="B19" s="4"/>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" t="s">
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
         <v>22</v>
       </c>
+      <c r="B19" s="4">
+        <f>(B9*B15-B8*B16)/(B15-B16)</f>
+        <v>-2.50000000000000711</v>
+      </c>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+    </row>
+    <row r="20" spans="2:2">
       <c r="B20" s="4"/>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="4">
-        <f>B14*B$17+B$18</f>
-        <v>4.148992260866180004E-11</v>
-      </c>
+      <c r="B21" s="4"/>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
         <v>24</v>
       </c>
       <c r="B22" s="4">
-        <f>B15*B$17+B$18</f>
-        <v>10.0000000002074998</v>
-      </c>
-    </row>
-    <row r="23" spans="2:2">
-      <c r="B23" s="4"/>
+        <f>B15*B$18+B$19</f>
+        <v>3.532996117883158149E-11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" s="4">
+        <f>B16*B$18+B$19</f>
+        <v>10.0000000001766889</v>
+      </c>
     </row>
     <row r="24" spans="2:2">
       <c r="B24" s="4"/>
@@ -801,12 +780,15 @@
     </row>
     <row r="34" spans="2:2">
       <c r="B34" s="4"/>
+    </row>
+    <row r="35" spans="2:2">
+      <c r="B35" s="4"/>
     </row>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1638791020" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1638877689" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -815,16 +797,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1638791020" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1638791020" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1638791020" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1638791020" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1638877689" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1638877689" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1638877689" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1638877689" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1638791020" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1638877689" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -848,7 +830,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="3" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="n">
         <v>150</v>
@@ -859,7 +841,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>150</v>
@@ -870,79 +852,79 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>3.29999999999999982</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>4</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>20</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B6" s="2" t="n">
         <v>4096</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>0</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>250</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B9" s="2" t="n">
         <v>128</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="2:2">
@@ -950,43 +932,43 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B11" s="4">
         <f>B2/1000</f>
         <v>0.15</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B12" s="4">
         <f>B4*B11</f>
         <v>0.6</v>
       </c>
       <c r="C12" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B13" s="4">
         <f>B5*B11</f>
         <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B14" s="2">
         <f>B12*B6*B9/B3</f>
@@ -995,7 +977,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B15" s="2">
         <f>B13*B6*B9/B3</f>
@@ -1007,7 +989,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B17" s="5">
         <f>(B8-B7)/(B15-B14)</f>
@@ -1016,7 +998,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B18" s="4">
         <f>(B8*B14-B7*B15)/(B14-B15)</f>
@@ -1028,13 +1010,13 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B20" s="4"/>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B21" s="4">
         <f>B14*B$17+B$18</f>
@@ -1043,7 +1025,7 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B22" s="4">
         <f>B15*B$17+B$18</f>
@@ -1054,7 +1036,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1638791020" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1638877689" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1063,16 +1045,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1638791020" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1638791020" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1638791020" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1638791020" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1638877689" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1638877689" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1638877689" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1638877689" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1638791020" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1638877689" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -1097,7 +1079,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="3" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="n">
         <v>100000</v>
@@ -1108,7 +1090,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>10000</v>
@@ -1119,79 +1101,79 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>3.29999999999999982</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>0</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>12</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B6" s="2" t="n">
         <v>4096</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>0</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>12</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B9" s="2" t="n">
         <v>128</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="2:2">
@@ -1199,43 +1181,43 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B11" s="4">
         <f>B2/(B1+B2)</f>
         <v>0.0909090909090909172</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B12" s="4">
         <f>B4*B11</f>
         <v>0</v>
       </c>
       <c r="C12" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B13" s="4">
         <f>B5*B11</f>
         <v>1.09090909090909193</v>
       </c>
       <c r="C13" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B14" s="2">
         <f>B12*B6*B9/B3</f>
@@ -1244,7 +1226,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B15" s="2">
         <f>B13*B6*B9/B3</f>
@@ -1256,7 +1238,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B17" s="5">
         <f>(B8-B7)/(B15-B14)</f>
@@ -1265,7 +1247,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B18" s="4">
         <f>(B8*B14-B7*B15)/(B14-B15)</f>
@@ -1277,13 +1259,13 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B20" s="4"/>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B21" s="4">
         <f>B14*B$17+B$18</f>
@@ -1292,7 +1274,7 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B22" s="4">
         <f>B15*B$17+B$18</f>
@@ -1303,7 +1285,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1638791020" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1638877689" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1312,16 +1294,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1638791020" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1638791020" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1638791020" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1638791020" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1638877689" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1638877689" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1638877689" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1638877689" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1638791020" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1638877689" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>

<commit_message>
Save point for u8g adaptation
</commit_message>
<xml_diff>
--- a/utilities/Dividers_calculator.xlsx
+++ b/utilities/Dividers_calculator.xlsx
@@ -5,7 +5,7 @@
   <fileSharing readOnlyRecommended="0" userName="alexe"/>
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0" xWindow="240" yWindow="60" windowWidth="0" windowHeight="0" tabRatio="500"/>
+    <workbookView activeTab="1" xWindow="240" yWindow="60" windowWidth="0" windowHeight="0" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="1-5 V" sheetId="1" r:id="rId4"/>
@@ -15,10 +15,10 @@
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1638877689" val="982" rev="124" revOS="4" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1638877689" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1638877689" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1638877689"/>
+      <pm:revision xmlns:pm="smNativeData" day="1641902781" val="982" rev="124" revOS="4" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1641902781" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1641902781" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1641902781"/>
     </ext>
   </extLst>
 </workbook>
@@ -136,7 +136,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1638877689" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1641902781" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -153,7 +153,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1638877689" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1641902781" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default" weight="bold"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -175,7 +175,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1638877689" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1641902781" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -197,7 +197,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1638877689"/>
+          <pm:border xmlns:pm="smNativeData" id="1641902781"/>
         </ext>
       </extLst>
     </border>
@@ -216,7 +216,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1638877689"/>
+          <pm:border xmlns:pm="smNativeData" id="1641902781"/>
         </ext>
       </extLst>
     </border>
@@ -239,7 +239,7 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1638877689" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1641902781" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
     </ext>
@@ -505,7 +505,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="normal" workbookViewId="0">
+    <sheetView view="normal" workbookViewId="0">
       <selection activeCell="E11" sqref="E11:F16"/>
     </sheetView>
   </sheetViews>
@@ -788,7 +788,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1638877689" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1641902781" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -797,16 +797,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1638877689" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1638877689" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1638877689" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1638877689" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1641902781" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1641902781" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1641902781" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1641902781" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1638877689" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1641902781" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -819,8 +819,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView view="normal" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" view="normal" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="13.45"/>
@@ -910,7 +910,7 @@
         <v>12</v>
       </c>
       <c r="B8" s="1" t="n">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>11</v>
@@ -993,7 +993,7 @@
       </c>
       <c r="B17" s="5">
         <f>(B8-B7)/(B15-B14)</f>
-        <v>0.000655651092529296164</v>
+        <v>0.000524520874023436967</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -1002,7 +1002,7 @@
       </c>
       <c r="B18" s="4">
         <f>(B8*B14-B7*B15)/(B14-B15)</f>
-        <v>-62.4999999999998721</v>
+        <v>-49.9999999999999929</v>
       </c>
     </row>
     <row r="19" spans="2:2">
@@ -1020,7 +1020,7 @@
       </c>
       <c r="B21" s="4">
         <f>B14*B$17+B$18</f>
-        <v>-2.820144118231837638E-11</v>
+        <v>-4.170175316176027991E-11</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -1029,14 +1029,14 @@
       </c>
       <c r="B22" s="4">
         <f>B15*B$17+B$18</f>
-        <v>249.999999999859142</v>
+        <v>199.99999999979201</v>
       </c>
     </row>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1638877689" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1641902781" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1045,16 +1045,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1638877689" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1638877689" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1638877689" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1638877689" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1641902781" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1641902781" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1641902781" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1641902781" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1638877689" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1641902781" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -1285,7 +1285,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1638877689" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1641902781" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1294,16 +1294,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1638877689" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1638877689" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1638877689" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1638877689" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1641902781" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1641902781" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1641902781" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1641902781" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1638877689" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1641902781" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>